<commit_message>
update sem gse ismt 2
</commit_message>
<xml_diff>
--- a/3_output/tablas/ajust_table_apbi.xlsx
+++ b/3_output/tablas/ajust_table_apbi.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>73.53729552766163</v>
       </c>
     </row>
     <row r="3">
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.9167350811896852</v>
       </c>
     </row>
     <row r="4">
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.05918277294611446</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.2246367943859071</v>
+        <v>0.373696506396882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update general recta final
</commit_message>
<xml_diff>
--- a/3_output/tablas/ajust_table_apbi.xlsx
+++ b/3_output/tablas/ajust_table_apbi.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>73.53729552766163</v>
+        <v>73.58335264412017</v>
       </c>
     </row>
     <row r="3">
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.9167350811896852</v>
+        <v>0.916654408844484</v>
       </c>
     </row>
     <row r="4">
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.05918277294611446</v>
+        <v>0.05921143599821604</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.373696506396882</v>
+        <v>0.3707876469228513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
msem con homogeneidad (sd)
</commit_message>
<xml_diff>
--- a/3_output/tablas/ajust_table_apbi.xlsx
+++ b/3_output/tablas/ajust_table_apbi.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>76.67380947660058</v>
+        <v>53.40575035845904</v>
       </c>
     </row>
     <row r="3">
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.9112725748431727</v>
+        <v>0.943946663536994</v>
       </c>
     </row>
     <row r="4">
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.06133949882556679</v>
+        <v>0.05458037482045512</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.3788847875922234</v>
+        <v>0.3756374367841092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>